<commit_message>
cambios realizados en sustentacion aplicados
</commit_message>
<xml_diff>
--- a/Seguros.xlsx
+++ b/Seguros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angeldvvp\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7750ac9e68e6bcb0/Documentos/PruebaChubbSegurosADVP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DD01966-9E5D-49C2-81E9-F73B9D0B39A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{C99DA352-0560-49BC-B7EB-9E914BB6294F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>NMBRSEGURO</t>
   </si>
@@ -51,25 +51,43 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>PRUEBA</t>
-  </si>
-  <si>
-    <t>CDS231</t>
-  </si>
-  <si>
     <t>ANGEL</t>
   </si>
   <si>
-    <t>PREUAB2</t>
-  </si>
-  <si>
-    <t>CDS2111|</t>
+    <t>Seguro de Incendio</t>
+  </si>
+  <si>
+    <t>ADKF123454</t>
+  </si>
+  <si>
+    <t>Seguro de Responsabilidad Civil</t>
+  </si>
+  <si>
+    <t>AJSM323422</t>
+  </si>
+  <si>
+    <t>Seguro Funerario</t>
+  </si>
+  <si>
+    <t>Kdma458155</t>
+  </si>
+  <si>
+    <t>Seguro Medico Plus</t>
+  </si>
+  <si>
+    <t>PLSM234333</t>
+  </si>
+  <si>
+    <t>Seguro Automotriz</t>
+  </si>
+  <si>
+    <t>ATRUD123443</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -118,10 +136,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -159,7 +181,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -265,7 +287,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -407,21 +429,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -451,16 +476,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="D2">
-        <v>50</v>
+        <v>42.5</v>
       </c>
       <c r="E2">
         <v>22</v>
@@ -469,7 +494,7 @@
         <v>50</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -483,10 +508,10 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D3">
-        <v>30</v>
+        <v>20.3</v>
       </c>
       <c r="E3">
         <v>18</v>
@@ -495,9 +520,87 @@
         <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>50000</v>
+      </c>
+      <c r="D4">
+        <v>35.619999999999997</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>99</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>60000</v>
+      </c>
+      <c r="D5">
+        <v>43.6</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>80</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>70000</v>
+      </c>
+      <c r="D6">
+        <v>60.5</v>
+      </c>
+      <c r="E6">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>70</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6">
         <v>1</v>
       </c>
     </row>

</xml_diff>